<commit_message>
add a pythonAPI for sector analysis, rename the py API directory
</commit_message>
<xml_diff>
--- a/finfun-ts/backend/src/sector_analysis_debug.xlsx
+++ b/finfun-ts/backend/src/sector_analysis_debug.xlsx
@@ -434,7 +434,7 @@
         <v>Communication Services</v>
       </c>
       <c r="C2">
-        <v>0.005</v>
+        <v>0.0049</v>
       </c>
       <c r="D2">
         <v>0.30857</v>
@@ -443,10 +443,10 @@
         <v>8.254</v>
       </c>
       <c r="F2">
-        <v>19.296875</v>
+        <v>19.167412</v>
       </c>
       <c r="G2">
-        <v>0.16493600579570153</v>
+        <v>0.1705385172663608</v>
       </c>
     </row>
     <row r="3">
@@ -457,7 +457,7 @@
         <v>Technology</v>
       </c>
       <c r="C3">
-        <v>0.0053</v>
+        <v>0.0052</v>
       </c>
       <c r="D3">
         <v>0.24301</v>
@@ -466,10 +466,10 @@
         <v>146.994</v>
       </c>
       <c r="F3">
-        <v>24.092659</v>
+        <v>24.169674</v>
       </c>
       <c r="G3">
-        <v>0.2302575932333718</v>
+        <v>0.22779700115340262</v>
       </c>
     </row>
     <row r="4">
@@ -480,7 +480,7 @@
         <v>Communication Services</v>
       </c>
       <c r="C4">
-        <v>0.0033000002</v>
+        <v>0.0032</v>
       </c>
       <c r="D4">
         <v>0.39113998</v>
@@ -489,10 +489,10 @@
         <v>26.763</v>
       </c>
       <c r="F4">
-        <v>25.388144</v>
+        <v>25.592491</v>
       </c>
       <c r="G4">
-        <v>0.13306609439743008</v>
+        <v>0.12608818884884798</v>
       </c>
     </row>
     <row r="5">
@@ -503,7 +503,7 @@
         <v>Technology</v>
       </c>
       <c r="C5">
-        <v>0.0074</v>
+        <v>0.0072000003</v>
       </c>
       <c r="D5">
         <v>0.35789</v>
@@ -512,10 +512,10 @@
         <v>32.626</v>
       </c>
       <c r="F5">
-        <v>30.815386</v>
+        <v>30.79331</v>
       </c>
       <c r="G5">
-        <v>0.016355289847336446</v>
+        <v>0.01705989110707806</v>
       </c>
     </row>
   </sheetData>
@@ -563,7 +563,7 @@
         <v>Communication Services</v>
       </c>
       <c r="C2">
-        <v>0.005</v>
+        <v>0.0049</v>
       </c>
       <c r="D2">
         <v>0.30857</v>
@@ -572,10 +572,10 @@
         <v>8.254</v>
       </c>
       <c r="F2">
-        <v>19.296875</v>
+        <v>19.167412</v>
       </c>
       <c r="G2">
-        <v>0.16493600579570153</v>
+        <v>0.1705385172663608</v>
       </c>
     </row>
     <row r="3">
@@ -586,7 +586,7 @@
         <v>Communication Services</v>
       </c>
       <c r="C3">
-        <v>0.005</v>
+        <v>0.0049</v>
       </c>
       <c r="D3">
         <v>0.30857</v>
@@ -595,10 +595,10 @@
         <v>8.254</v>
       </c>
       <c r="F3">
-        <v>19.439106</v>
+        <v>19.31285</v>
       </c>
       <c r="G3">
-        <v>0.1663632007666507</v>
+        <v>0.1717776712985146</v>
       </c>
     </row>
     <row r="4">
@@ -609,7 +609,7 @@
         <v>Communication Services</v>
       </c>
       <c r="C4">
-        <v>0.0405</v>
+        <v>0.0399</v>
       </c>
       <c r="D4">
         <v>0.096429996</v>
@@ -618,10 +618,10 @@
         <v>119.246</v>
       </c>
       <c r="F4">
-        <v>12.227678</v>
+        <v>12.410714</v>
       </c>
       <c r="G4">
-        <v>0.05649328281088531</v>
+        <v>0.04236996210816398</v>
       </c>
     </row>
     <row r="5">
@@ -641,10 +641,10 @@
         <v>465.632</v>
       </c>
       <c r="F5">
-        <v>11.490498</v>
+        <v>11.075182</v>
       </c>
       <c r="G5">
-        <v>0.059328238685763986</v>
+        <v>0.09332814716514899</v>
       </c>
     </row>
     <row r="6">
@@ -664,10 +664,10 @@
         <v>113.542</v>
       </c>
       <c r="F6">
-        <v>7.979452</v>
+        <v>7.892694</v>
       </c>
       <c r="G6">
-        <v>0.22864709777091147</v>
+        <v>0.2370337673802693</v>
       </c>
     </row>
     <row r="7">
@@ -678,7 +678,7 @@
         <v>Communication Services</v>
       </c>
       <c r="C7">
-        <v>0.0052</v>
+        <v>0.0053</v>
       </c>
       <c r="D7">
         <v>0.15021</v>
@@ -687,10 +687,10 @@
         <v>34.732</v>
       </c>
       <c r="F7">
-        <v>17.222744</v>
+        <v>16.855803</v>
       </c>
       <c r="G7">
-        <v>0.1281305637982196</v>
+        <v>0.14670623145400594</v>
       </c>
     </row>
     <row r="8">
@@ -710,10 +710,10 @@
         <v>68.321</v>
       </c>
       <c r="F8">
-        <v>14.959785</v>
+        <v>14.729222</v>
       </c>
       <c r="G8">
-        <v>0.050051072522982715</v>
+        <v>0.06469186244467151</v>
       </c>
     </row>
     <row r="9">
@@ -733,10 +733,10 @@
         <v>68.321</v>
       </c>
       <c r="F9">
-        <v>21.765959</v>
+        <v>21.395744</v>
       </c>
       <c r="G9">
-        <v>0.07000000000000002</v>
+        <v>0.0858181818181818</v>
       </c>
     </row>
     <row r="10">
@@ -747,7 +747,7 @@
         <v>Communication Services</v>
       </c>
       <c r="C10">
-        <v>0.055</v>
+        <v>0.0551</v>
       </c>
       <c r="D10">
         <v>0.05485</v>
@@ -756,10 +756,10 @@
         <v>113.87</v>
       </c>
       <c r="F10">
-        <v>8.901818</v>
+        <v>8.712727</v>
       </c>
       <c r="G10">
-        <v>0.25930408472012095</v>
+        <v>0.27503782148260203</v>
       </c>
     </row>
     <row r="11">
@@ -779,10 +779,10 @@
         <v>393.218</v>
       </c>
       <c r="F11">
-        <v>59.099174</v>
+        <v>56.690083</v>
       </c>
       <c r="G11">
-        <v>0.09337559429477015</v>
+        <v>0.1303328050713154</v>
       </c>
     </row>
     <row r="12">
@@ -793,7 +793,7 @@
         <v>Communication Services</v>
       </c>
       <c r="C12">
-        <v>0.0033000002</v>
+        <v>0.0032</v>
       </c>
       <c r="D12">
         <v>0.39113998</v>
@@ -802,10 +802,10 @@
         <v>26.763</v>
       </c>
       <c r="F12">
-        <v>25.388144</v>
+        <v>25.592491</v>
       </c>
       <c r="G12">
-        <v>0.13306609439743008</v>
+        <v>0.12608818884884798</v>
       </c>
     </row>
     <row r="13">
@@ -825,10 +825,10 @@
         <v>72.513</v>
       </c>
       <c r="F13">
-        <v>50.949112</v>
+        <v>50.76661</v>
       </c>
       <c r="G13">
-        <v>0.0001650478226066378</v>
+        <v>0.007138686251449583</v>
       </c>
     </row>
     <row r="14">
@@ -839,7 +839,7 @@
         <v>Communication Services</v>
       </c>
       <c r="C14">
-        <v>0.0072000003</v>
+        <v>0.0070999996</v>
       </c>
       <c r="D14">
         <v>0.04743</v>
@@ -848,10 +848,10 @@
         <v>32.188</v>
       </c>
       <c r="F14">
-        <v>26.650946</v>
+        <v>26.64151</v>
       </c>
       <c r="G14">
-        <v>0.07950472466601503</v>
+        <v>0.07983056370153153</v>
       </c>
     </row>
     <row r="15">
@@ -862,7 +862,7 @@
         <v>Communication Services</v>
       </c>
       <c r="C15">
-        <v>0.0062</v>
+        <v>0.0061000003</v>
       </c>
       <c r="D15">
         <v>0.04743</v>
@@ -871,10 +871,10 @@
         <v>32.188</v>
       </c>
       <c r="F15">
-        <v>39.707317</v>
+        <v>39.90244</v>
       </c>
       <c r="G15">
-        <v>0.07631205673758859</v>
+        <v>0.07177304964539011</v>
       </c>
     </row>
     <row r="16">
@@ -885,7 +885,7 @@
         <v>Communication Services</v>
       </c>
       <c r="C16">
-        <v>0.0383</v>
+        <v>0.0381</v>
       </c>
       <c r="D16">
         <v>0.09205</v>
@@ -894,10 +894,10 @@
         <v>129.051</v>
       </c>
       <c r="F16">
-        <v>8.59375</v>
+        <v>8.5</v>
       </c>
       <c r="G16">
-        <v>0.3060747663551402</v>
+        <v>0.31364485981308415</v>
       </c>
     </row>
     <row r="17">
@@ -908,7 +908,7 @@
         <v>Communication Services</v>
       </c>
       <c r="C17">
-        <v>0.0167</v>
+        <v>0.0165</v>
       </c>
       <c r="D17">
         <v>-0.19094999</v>
@@ -917,10 +917,10 @@
         <v>91.724</v>
       </c>
       <c r="F17">
-        <v>7.3803678</v>
+        <v>7.423313</v>
       </c>
       <c r="G17">
-        <v>0.07816091954022998</v>
+        <v>0.07279693486590046</v>
       </c>
     </row>
     <row r="18">
@@ -940,10 +940,10 @@
         <v>199.152</v>
       </c>
       <c r="F18">
-        <v>22.807873</v>
+        <v>22.699156</v>
       </c>
       <c r="G18">
-        <v>0.11982350175413213</v>
+        <v>0.12401895186082686</v>
       </c>
     </row>
     <row r="19">
@@ -963,10 +963,10 @@
         <v>192.071</v>
       </c>
       <c r="F19">
-        <v>28.86097</v>
+        <v>28.862244</v>
       </c>
       <c r="G19">
-        <v>0.06026248027244784</v>
+        <v>0.06022094858376942</v>
       </c>
     </row>
     <row r="20">
@@ -986,10 +986,10 @@
         <v>30.107</v>
       </c>
       <c r="F20">
-        <v>49.05864</v>
+        <v>48.70679</v>
       </c>
       <c r="G20">
-        <v>0.11245742364174445</v>
+        <v>0.11882293818750349</v>
       </c>
     </row>
     <row r="21">
@@ -1000,7 +1000,7 @@
         <v>Communication Services</v>
       </c>
       <c r="C21">
-        <v>0.0626</v>
+        <v>0.0616</v>
       </c>
       <c r="D21">
         <v>0.13144</v>
@@ -1009,10 +1009,10 @@
         <v>169.089</v>
       </c>
       <c r="F21">
-        <v>9.196617</v>
+        <v>9.293869</v>
       </c>
       <c r="G21">
-        <v>0.08150337837837837</v>
+        <v>0.07179054054054052</v>
       </c>
     </row>
     <row r="22">
@@ -1023,7 +1023,7 @@
         <v>Communication Services</v>
       </c>
       <c r="C22">
-        <v>0.0091</v>
+        <v>0.0088</v>
       </c>
       <c r="D22">
         <v>0.09475</v>
@@ -1032,10 +1032,10 @@
         <v>39.432</v>
       </c>
       <c r="F22">
-        <v>21.817476</v>
+        <v>21.949514</v>
       </c>
       <c r="G22">
-        <v>0.052853409761443114</v>
+        <v>0.04712130152575225</v>
       </c>
     </row>
     <row r="23">
@@ -1055,10 +1055,10 @@
         <v>106.412</v>
       </c>
       <c r="F23">
-        <v>-73.46154</v>
+        <v>-76.692314</v>
       </c>
       <c r="G23">
-        <v>0.24803149606299202</v>
+        <v>0.21496062992125975</v>
       </c>
     </row>
   </sheetData>

</xml_diff>